<commit_message>
update schema to test
</commit_message>
<xml_diff>
--- a/FakeApiDataTableColumns.xlsx
+++ b/FakeApiDataTableColumns.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>UserDetails</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>AllowedDate</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>SessionId</t>
+  </si>
+  <si>
+    <t>OTP</t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,7 +447,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,14 +535,20 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>